<commit_message>
Update Progress report and add STD
</commit_message>
<xml_diff>
--- a/Doc/iteration2/CS673_ProgressReport_team2.xlsx
+++ b/Doc/iteration2/CS673_ProgressReport_team2.xlsx
@@ -385,11 +385,13 @@
     <t>06/08 - 06/14</t>
   </si>
   <si>
-    <t>4 - Added tests for SortBySelect &amp; NavMenuItems
+    <t>0 - Did research about Nonfunctional testing
+4 - Added tests for SortBySelect &amp; NavMenuItems
 6 - Created a Pull Request</t>
   </si>
   <si>
-    <t>- SPPP: updated Quality Assurance Plan part</t>
+    <t>- SPPP: updated Quality Assurance Plan part
+- STD: Manual tests and automated Testing reports</t>
   </si>
   <si>
     <t>- Write more tests
@@ -8958,11 +8960,11 @@
       </c>
       <c r="C8" s="9">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D8" s="9">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E8" s="8">
         <v>1.0</v>
@@ -8970,13 +8972,19 @@
       <c r="F8" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="G8" s="6"/>
+      <c r="G8" s="7">
+        <v>3.0</v>
+      </c>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
       <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
+      <c r="K8" s="7">
+        <v>1.0</v>
+      </c>
       <c r="L8" s="6"/>
-      <c r="M8" s="6"/>
+      <c r="M8" s="7">
+        <v>1.0</v>
+      </c>
       <c r="N8" s="6"/>
       <c r="O8" s="7" t="s">
         <v>85</v>
@@ -8986,7 +8994,9 @@
       <c r="R8" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="S8" s="6"/>
+      <c r="S8" s="7">
+        <v>20.0</v>
+      </c>
       <c r="T8" s="6"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">

</xml_diff>